<commit_message>
CANS-236. Add caregiver domains
</commit_message>
<xml_diff>
--- a/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank.xlsx
+++ b/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/metquota/cwds/cans-api/tools/instrument-parser/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{13F83F64-9041-DC42-B855-FE1BC73DA621}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{507E7E29-CA27-4A4B-9A11-9E699FFFAA26}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39880" yWindow="1620" windowWidth="28800" windowHeight="16680" tabRatio="555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37680" yWindow="5600" windowWidth="28800" windowHeight="16680" tabRatio="555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Domains" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="782">
   <si>
     <t>Domain_ID</t>
   </si>
@@ -3140,6 +3140,9 @@
   </si>
   <si>
     <t>SLEEP_CHILD</t>
+  </si>
+  <si>
+    <t>Is_A_Caregiver_Domain</t>
   </si>
 </sst>
 </file>
@@ -3209,7 +3212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3235,6 +3238,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3549,10 +3555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -3562,10 +3568,12 @@
     <col min="3" max="3" width="12.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="5" customWidth="1"/>
-    <col min="6" max="16384" width="8.83203125" style="5"/>
+    <col min="6" max="7" width="8.83203125" style="5"/>
+    <col min="8" max="8" width="12.6640625" style="10" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15" ht="31" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3587,29 +3595,32 @@
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="11" t="s">
+        <v>781</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>398</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3628,23 +3639,23 @@
       <c r="G2" s="5">
         <v>1</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:15">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -3663,23 +3674,23 @@
       <c r="G3" s="5">
         <v>1</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -3698,23 +3709,23 @@
       <c r="G4" s="5">
         <v>1</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -3733,23 +3744,23 @@
       <c r="G5" s="5">
         <v>1</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>377</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -3768,23 +3779,23 @@
       <c r="G6" s="5">
         <v>1</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="I6" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="O6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:15">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -3806,23 +3817,26 @@
       <c r="G7" s="5">
         <v>1</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="10">
+        <v>1</v>
+      </c>
+      <c r="I7" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="J7" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="L7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="O7" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:15">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -3844,17 +3858,17 @@
       <c r="G8" s="5">
         <v>1</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="M8" s="5" t="s">
         <v>399</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="N8" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="O8" s="5" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:15">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -3867,23 +3881,23 @@
       <c r="F9" s="5">
         <v>1</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="I9" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="J9" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="O9" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:15">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -3896,23 +3910,23 @@
       <c r="F10" s="5">
         <v>1</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="O10" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:15">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -3925,23 +3939,23 @@
       <c r="F11" s="5">
         <v>1</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>365</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="K11" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="O11" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:15">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -3954,23 +3968,23 @@
       <c r="F12" s="5">
         <v>1</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>366</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="K12" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="O12" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:15">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -3983,23 +3997,23 @@
       <c r="F13" s="5">
         <v>1</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="I13" s="5" t="s">
         <v>381</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="J13" s="5" t="s">
         <v>382</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
         <v>383</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="L13" s="5" t="s">
         <v>384</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="O13" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:15">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -4012,19 +4026,19 @@
       <c r="F14" s="5">
         <v>1</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="I14" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="J14" s="5" t="s">
         <v>389</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="K14" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="L14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="O14" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -4037,7 +4051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q2" sqref="Q2"/>
       <selection pane="bottomLeft" activeCell="M22" sqref="M22"/>

</xml_diff>

<commit_message>
CANS-314: additional spelling mistakes in assessment fixed
</commit_message>
<xml_diff>
--- a/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank.xlsx
+++ b/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank.xlsx
@@ -355,9 +355,6 @@
     <t>There is no evidence that the child/youth has experienced physical abuse.</t>
   </si>
   <si>
-    <t xml:space="preserve">Child/youth has experienced or there is a suspicion that they experienced physical abuse – mild to severe, or repeated physical abuse with sufficient physical harm requiring medical treatment. </t>
-  </si>
-  <si>
     <t>T03</t>
   </si>
   <si>
@@ -967,9 +964,6 @@
   </si>
   <si>
     <t>Action or intervention is required to ensure that the identified need is addressed; need is interfering with functioning. Concern in one or more areas of regulation: sleep, crying, feeding, tantrums, sensitivity to touch, noise, and environment. Referral to address self-regulation is needed.</t>
-  </si>
-  <si>
-    <t>Problems are dangerous or disabling; requires immediate and/or intensive action .Concern in two or more areas of regulation, including but not limited to: difficulties in breathing, body movements, crying, sleeping, feeding, attention, ability to self soothe, and/or sensitivity to environmental stressors.</t>
   </si>
   <si>
     <t>Self-Harm</t>
@@ -1353,9 +1347,6 @@
     <t>Is_A_Caregiver_Domain</t>
   </si>
   <si>
-    <t>Terrorism is defined as &amp;quot;the calculated use of violence or the threat of violence to inculcate fear, intended to coerce or to intimidate governments or societies in the pursuit of goals that are generally political, religious or ideological.&amp;quot; Terrorism includes attacks by individuals acting in isolation (e.g. sniper attacks).</t>
-  </si>
-  <si>
     <t xml:space="preserve">• Does the child/youth exhibit behaviors that are unusual or difficult to understand?
 • Does the child/youth experience hallucinations or delusions, bizarre behavior?
 • Are the unusual behaviors, hallucinations or delusions interfering with the youth's functioning?
@@ -1435,14 +1426,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">For children birth to 5 years old, consider the following:
-• Action level '0': Child has a prosocial or &amp;quot;easy&amp;quot; temperament and, if old enough, is interested and effective at initiating relationships with other children or adults. If still an infant, child exhibits anticipatory behavior when fed or held.
-• Action level '1': Child has formed a positive interpersonal relationship with at least one non-caregiver. Child responds positively to social initiations by adults but may not initiate such interactions by themselves.
-• Action level '2': Child may be shy or uninterested in forming relationships with others, or – if still an infant-child may have a temperament that makes attachment to others a challenge.
-• Action level '3': Child with no known interpersonal strengths. Child does not exhibit any age-appropriate social gestures (e.g. Social smile, cooperative play, responsiveness to social initiations by non-caregivers). An infant that consistently exhibits gaze aversion would be rated here.
-</t>
-  </si>
-  <si>
     <t>This item is used to evaluate the nature of the school's relationship with the youth and family, as well as, the level of support the youth receives from the school. Rate according to how much the school is an effective partner in promoting youth's functioning and addressing youth's needs in school.</t>
   </si>
   <si>
@@ -1711,12 +1694,6 @@
     <t xml:space="preserve">This item describes whether or not the child/ youth has experienced sexual abuse. </t>
   </si>
   <si>
-    <t xml:space="preserve">Child/youth has experienced sexual abuse, or there is a suspicion that they have experienced sexual abuse – including single or multiple episodes, or chronic over an extended period of time. The abuse may have involved penetration, multiple perpetrators, and/or associated physical injury. Child/youth with exposure to secondary sexual abuse (e.g., witnessing sexual abuse, having a sibling sexually abused) should be rated here. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">This item describes whether or not the child/youth has experienced verbal and/or nonverbal emotional abuse, including belittling, shaming, and humiliating a child/youth, calling names, making negative comparisons to others, or telling a child/youth that they are, &amp;quot;no good.&amp;quot; This item includes both &amp;quot;emotional abuse,&amp;quot; which would include psychological maltreatment such as insults or humiliation towards a child and &amp;quot;emotional neglect,&amp;quot; described as the denial of emotional attention and/or support from caregivers. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Child/youth has experienced emotional abuse, or there is a suspicion that they have experienced emotional abuse (mild to severe, for any length of time) including: insults or occasionally being referred to in a derogatory manner by caregivers, being denied emotional attention or completely ignored, or threatened/terrorized by others. </t>
   </si>
   <si>
@@ -1727,9 +1704,6 @@
   </si>
   <si>
     <t>This item takes into account the impact of the event on the child/youth. It describes experiences in which the child/youth is subjected to medical procedures that are experienced as upsetting and overwhelming. A child/youth born with physical deformities who is subjected to multiple surgeries could be included. A child/ youth who must experience chemotherapy or radiation could also be included. Children/youth who experience an accident and require immediate medical intervention that results in on-going physical limitations or deformities (e.g., burn victims) could be included here. Common medical procedures, which are generally not welcome or pleasant but are also not emotionally or psychologically overwhelming for children (e.g., shots, pills) would generally not be rated here.</t>
-  </si>
-  <si>
-    <t>Child/youth has witnessed, or there is a suspicion that they witnessed family violence – single, repeated, or severe episodes. This includes episodes of family violence but no significant injuries (i.e. requiring emergency medical attention) and episodes in which significant injuries have occurred as a direct result of the violence.</t>
   </si>
   <si>
     <t>This item describes the exposure to incidents of violence the youth has witnessed or experienced in his/her community. This includes witnessing violence at the child/youth's school or educational setting.</t>
@@ -2261,9 +2235,6 @@
     <t xml:space="preserve">Problems are dangerous or disabling; requires immediate and/or intensive action. Child/youth has severe to profound intellectual disability (FSIQ, if available, less than 55) and/or Autism Spectrum Disorder with marked to profound deficits in adaptive functioning in one or more areas: communication, social participation and independent living across multiple environments. </t>
   </si>
   <si>
-    <t xml:space="preserve">Problems are dangerous or disabling; requires immediate and/or intensive action. Child/youth makes decisions that would likely result in significant physical harm to self or others. Therefore, youth requires intense and constant supervision, over and above that expected for the child/yo uth's age. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Problems are dangerous or disabling; requires immediate and/or intensive action. Child/youth is having severe achievement problems. The child/youth may be failing most subjects or has been retained (held back) a grade level. Child/youth might be more than one year behind same-age peers in school achievement. </t>
   </si>
   <si>
@@ -2582,18 +2553,12 @@
     <t xml:space="preserve">No current need; no need for action or intervention. This may be strength of the caregiver. Caregiver is emotionally empathic and attends to the child's emotional needs. </t>
   </si>
   <si>
-    <t xml:space="preserve">Problems are dangerous or disabling; requires immediate and/or intensive action The caregiver has significant difficulties with emotional responsiveness. They are not empathic and rarely attends to the child's emotional needs. </t>
-  </si>
-  <si>
     <t xml:space="preserve">No current need; no need for action or intervention. This may be strength of the caregiver. There is no evidence that the caregiver has experienced trauma, OR there is evidence that the caregiver has adjusted well to their traumatic experiences. </t>
   </si>
   <si>
     <t xml:space="preserve">Identified need requires monitoring, watchful waiting, or preventive activities. This may be an opportunity for strength building. The caregiver has mild adjustment problems and exhibits some signs of distress, OR caregiver has a history of having difficulty adjusting to traumatic experiences. </t>
   </si>
   <si>
-    <t xml:space="preserve">Problems are dangerous or disabling; requires immediate and/or intensive action The caregiver has post-traumatic stress difficulties. Symptoms may include intrusive thoughts, hyper-vigilance, constant anxiety, and other common symptoms of Post-Traumatic Stress Disorder (PTSD). </t>
-  </si>
-  <si>
     <t xml:space="preserve">Problems are dangerous or disabling; requires immediate and/or intensive action The caregiver's hesitancy to engage with the formal helping system prohibits the family's engagement with the treatment team at this time. When this occurs, the development of an alternate treatment plan may be required. </t>
   </si>
   <si>
@@ -2628,6 +2593,41 @@
   </si>
   <si>
     <t>How did the child's birth weight compare to typical averages?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problems are dangerous or disabling; requires immediate and/or intensive action. Child/youth makes decisions that would likely result in significant physical harm to self or others. Therefore, youth requires intense and constant supervision, over and above that expected for the child/youth's age. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This item describes whether or not the child/youth has experienced verbal and/or nonverbal emotional abuse, including belittling, shaming, and humiliating a child/youth, calling names, making negative comparisons to others, or telling a child/youth that they are, "no good." This item includes both "emotional abuse," which would include psychological maltreatment such as insults or humiliation towards a child and "emotional neglect," described as the denial of emotional attention and/or support from caregivers. </t>
+  </si>
+  <si>
+    <t>Terrorism is defined as "the calculated use of violence or the threat of violence to inculcate fear, intended to coerce or to intimidate governments or societies in the pursuit of goals that are generally political, religious or ideological." Terrorism includes attacks by individuals acting in isolation (e.g. sniper attacks).</t>
+  </si>
+  <si>
+    <t>Problems are dangerous or disabling; requires immediate and/or intensive action. Concern in two or more areas of regulation, including but not limited to: difficulties in breathing, body movements, crying, sleeping, feeding, attention, ability to self soothe, and/or sensitivity to environmental stressors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problems are dangerous or disabling; requires immediate and/or intensive action. The caregiver has significant difficulties with emotional responsiveness. They are not empathic and rarely attends to the child's emotional needs. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problems are dangerous or disabling; requires immediate and/or intensive action. The caregiver has post-traumatic stress difficulties. Symptoms may include intrusive thoughts, hyper-vigilance, constant anxiety, and other common symptoms of Post-Traumatic Stress Disorder (PTSD). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Child/youth has experienced sexual abuse, or there is a suspicion that they have experienced sexual abuse - including single or multiple episodes, or chronic over an extended period of time. The abuse may have involved penetration, multiple perpetrators, and/or associated physical injury. Child/youth with exposure to secondary sexual abuse (e.g., witnessing sexual abuse, having a sibling sexually abused) should be rated here. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Child/youth has experienced or there is a suspicion that they experienced physical abuse - mild to severe, or repeated physical abuse with sufficient physical harm requiring medical treatment. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">For children birth to 5 years old, consider the following:
+• Action level '0': Child has a prosocial or "easy" temperament and, if old enough, is interested and effective at initiating relationships with other children or adults. If still an infant, child exhibits anticipatory behavior when fed or held.
+• Action level '1': Child has formed a positive interpersonal relationship with at least one non-caregiver. Child responds positively to social initiations by adults but may not initiate such interactions by themselves.
+• Action level '2': Child may be shy or uninterested in forming relationships with others, or - if still an infant-child may have a temperament that makes attachment to others a challenge.
+• Action level '3': Child with no known interpersonal strengths. Child does not exhibit any age-appropriate social gestures (e.g. Social smile, cooperative play, responsiveness to social initiations by non-caregivers). An infant that consistently exhibits gaze aversion would be rated here.
+</t>
+  </si>
+  <si>
+    <t>Child/youth has witnessed, or there is a suspicion that they witnessed family violence - single, repeated, or severe episodes. This includes episodes of family violence but no significant injuries (i.e. requiring emergency medical attention) and episodes in which significant injuries have occurred as a direct result of the violence.</t>
   </si>
 </sst>
 </file>
@@ -3040,16 +3040,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>197</v>
-      </c>
       <c r="E1" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -3058,28 +3058,28 @@
         <v>5</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -3087,28 +3087,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>518</v>
+        <v>511</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="G2" s="4">
         <v>1</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>12</v>
@@ -3122,28 +3122,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>207</v>
-      </c>
       <c r="G3" s="4">
         <v>1</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>12</v>
@@ -3157,28 +3157,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="G4" s="4">
         <v>1</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>12</v>
@@ -3192,28 +3192,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>514</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>515</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>521</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>522</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>210</v>
-      </c>
       <c r="K5" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>12</v>
@@ -3227,31 +3227,31 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>523</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="G6" s="4">
-        <v>1</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="L6" s="4" t="s">
-        <v>216</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>6</v>
@@ -3262,34 +3262,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>524</v>
-      </c>
-      <c r="F7" s="4">
-        <v>1</v>
-      </c>
-      <c r="G7" s="4">
-        <v>1</v>
-      </c>
-      <c r="H7" s="8">
-        <v>1</v>
-      </c>
-      <c r="I7" s="4" t="s">
+      <c r="J7" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>219</v>
-      </c>
       <c r="K7" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L7" s="4" t="s">
         <v>12</v>
@@ -3303,17 +3303,17 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>518</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>525</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>221</v>
-      </c>
       <c r="F8" s="4">
         <v>1</v>
       </c>
@@ -3321,13 +3321,13 @@
         <v>1</v>
       </c>
       <c r="M8" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="N8" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>229</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -3335,22 +3335,22 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
       </c>
       <c r="I9" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J9" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="K9" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>12</v>
@@ -3364,16 +3364,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>10</v>
@@ -3393,22 +3393,22 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
       </c>
       <c r="I11" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J11" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="K11" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>12</v>
@@ -3422,22 +3422,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="F12" s="4">
-        <v>1</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>236</v>
-      </c>
       <c r="J12" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="K12" s="4" t="s">
         <v>203</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>204</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>12</v>
@@ -3451,25 +3451,25 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
       </c>
       <c r="I13" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="K13" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="L13" s="4" t="s">
         <v>215</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>216</v>
       </c>
       <c r="O13" s="4" t="s">
         <v>6</v>
@@ -3480,22 +3480,22 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
       </c>
       <c r="I14" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>219</v>
-      </c>
       <c r="K14" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>12</v>
@@ -3513,10 +3513,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q2" sqref="Q2"/>
-      <selection pane="bottomLeft" activeCell="Y1" sqref="Y1:Y1048576"/>
+      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3545,7 +3545,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -3554,43 +3554,43 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="M1" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>4</v>
@@ -3605,16 +3605,16 @@
         <v>6</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -3628,28 +3628,28 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>649</v>
+        <v>642</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="S2" s="1">
         <v>1</v>
@@ -3672,22 +3672,22 @@
         <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>650</v>
+        <v>643</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>16</v>
@@ -3719,22 +3719,22 @@
         <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>699</v>
+        <v>691</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>776</v>
+        <v>766</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>700</v>
+        <v>692</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>19</v>
@@ -3766,22 +3766,22 @@
         <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>514</v>
+        <v>507</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>651</v>
+        <v>644</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>22</v>
@@ -3813,25 +3813,25 @@
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>701</v>
+        <v>693</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>702</v>
+        <v>694</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="Q6" s="1">
         <v>1</v>
@@ -3857,22 +3857,22 @@
         <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>704</v>
+        <v>696</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>705</v>
+        <v>697</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>27</v>
@@ -3898,22 +3898,22 @@
         <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>706</v>
+        <v>698</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>707</v>
+        <v>699</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>652</v>
+        <v>645</v>
       </c>
       <c r="N8" s="7">
         <v>1</v>
@@ -3945,22 +3945,22 @@
         <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>653</v>
+        <v>646</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>31</v>
@@ -3989,25 +3989,25 @@
         <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>654</v>
+        <v>647</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="Q10" s="1">
         <v>1</v>
@@ -4036,25 +4036,25 @@
         <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>708</v>
+        <v>700</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>655</v>
+        <v>648</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="Q11" s="1">
         <v>1</v>
@@ -4080,25 +4080,25 @@
         <v>37</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>709</v>
+        <v>701</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>710</v>
+        <v>702</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>656</v>
+        <v>649</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>777</v>
+        <v>767</v>
       </c>
       <c r="R12" s="1">
         <v>1</v>
@@ -4121,25 +4121,25 @@
         <v>38</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>657</v>
+        <v>650</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="R13" s="1">
         <v>1</v>
@@ -4165,25 +4165,25 @@
         <v>40</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>711</v>
+        <v>703</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="Q14" s="1">
         <v>1</v>
@@ -4206,28 +4206,28 @@
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>712</v>
+        <v>704</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>713</v>
+        <v>705</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>659</v>
+        <v>772</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="R15" s="1">
         <v>1</v>
@@ -4250,25 +4250,25 @@
         <v>41</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="O16" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>715</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>716</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>245</v>
       </c>
       <c r="R16" s="1">
         <v>1</v>
@@ -4291,25 +4291,25 @@
         <v>42</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>660</v>
+        <v>652</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="R17" s="1">
         <v>1</v>
@@ -4332,25 +4332,25 @@
         <v>43</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>717</v>
+        <v>709</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>718</v>
+        <v>710</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>661</v>
+        <v>653</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="R18" s="1">
         <v>1</v>
@@ -4376,25 +4376,25 @@
         <v>45</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>662</v>
+        <v>654</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="R19" s="1">
         <v>1</v>
@@ -4414,28 +4414,28 @@
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>719</v>
+        <v>711</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>663</v>
+        <v>655</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="R20" s="1">
         <v>1</v>
@@ -4455,31 +4455,31 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q21" s="1">
         <v>1</v>
@@ -4505,25 +4505,25 @@
         <v>47</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>720</v>
+        <v>712</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>721</v>
+        <v>713</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="R22" s="1">
         <v>1</v>
@@ -4549,25 +4549,25 @@
         <v>49</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>722</v>
+        <v>714</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>665</v>
+        <v>657</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="R23" s="1">
         <v>1</v>
@@ -4593,25 +4593,25 @@
         <v>50</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>723</v>
+        <v>715</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>666</v>
+        <v>658</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R24" s="1">
         <v>1</v>
@@ -4637,25 +4637,25 @@
         <v>51</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>724</v>
+        <v>716</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>725</v>
+        <v>717</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R25" s="1">
         <v>1</v>
@@ -4681,25 +4681,25 @@
         <v>52</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>726</v>
+        <v>718</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>727</v>
+        <v>719</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>667</v>
+        <v>659</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="R26" s="1">
         <v>1</v>
@@ -4725,25 +4725,25 @@
         <v>53</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>728</v>
+        <v>720</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>729</v>
+        <v>721</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="R27" s="1">
         <v>1</v>
@@ -4769,25 +4769,25 @@
         <v>54</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>730</v>
+        <v>722</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>668</v>
+        <v>660</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="R28" s="1">
         <v>1</v>
@@ -4816,25 +4816,25 @@
         <v>55</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>731</v>
+        <v>723</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>669</v>
+        <v>661</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R29" s="1">
         <v>1</v>
@@ -4860,25 +4860,25 @@
         <v>57</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>670</v>
+        <v>662</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="Q30" s="1">
         <v>1</v>
@@ -4907,25 +4907,25 @@
         <v>60</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>732</v>
+        <v>724</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>671</v>
+        <v>663</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Q31" s="1">
         <v>1</v>
@@ -4954,25 +4954,25 @@
         <v>62</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>672</v>
+        <v>664</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="Q32" s="1">
         <v>1</v>
@@ -5001,25 +5001,25 @@
         <v>64</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>733</v>
+        <v>725</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>734</v>
+        <v>726</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="Q33" s="1">
         <v>1</v>
@@ -5048,28 +5048,28 @@
         <v>66</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>570</v>
+        <v>563</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>405</v>
+        <v>780</v>
       </c>
       <c r="Q34" s="1">
         <v>1</v>
@@ -5095,28 +5095,28 @@
         <v>67</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="M35" s="7">
         <v>1</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="R35" s="1">
         <v>1</v>
@@ -5136,28 +5136,28 @@
         <v>35</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>68</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="R36" s="1">
         <v>1</v>
@@ -5180,25 +5180,25 @@
         <v>70</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>735</v>
+        <v>727</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="R37" s="1">
         <v>1</v>
@@ -5221,25 +5221,25 @@
         <v>71</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="R38" s="1">
         <v>1</v>
@@ -5262,25 +5262,25 @@
         <v>72</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="R39" s="1">
         <v>1</v>
@@ -5303,28 +5303,28 @@
         <v>73</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>736</v>
+        <v>728</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="R40" s="1">
         <v>1</v>
@@ -5350,25 +5350,25 @@
         <v>75</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>737</v>
+        <v>729</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="Q41" s="1">
         <v>1</v>
@@ -5397,25 +5397,25 @@
         <v>77</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>738</v>
+        <v>730</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q42" s="1">
         <v>1</v>
@@ -5444,25 +5444,25 @@
         <v>79</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>739</v>
+        <v>731</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Q43" s="1">
         <v>1</v>
@@ -5491,28 +5491,28 @@
         <v>81</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>740</v>
+        <v>732</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="Q44" s="1">
         <v>1</v>
@@ -5541,25 +5541,25 @@
         <v>83</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>741</v>
+        <v>733</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>630</v>
+        <v>623</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="Q45" s="1">
         <v>1</v>
@@ -5585,28 +5585,28 @@
         <v>84</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>742</v>
+        <v>734</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>743</v>
+        <v>735</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="Q46" s="1">
         <v>1</v>
@@ -5635,25 +5635,25 @@
         <v>45</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>744</v>
+        <v>736</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>684</v>
+        <v>676</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="Q47" s="1">
         <v>1</v>
@@ -5682,25 +5682,25 @@
         <v>87</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>746</v>
+        <v>738</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>685</v>
+        <v>677</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="Q48" s="1">
         <v>1</v>
@@ -5729,28 +5729,28 @@
         <v>28</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>89</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>747</v>
+        <v>739</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>686</v>
+        <v>678</v>
       </c>
       <c r="N49" s="7">
         <v>1</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Q49" s="1">
         <v>1</v>
@@ -5782,25 +5782,25 @@
         <v>91</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>687</v>
+        <v>679</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Q50" s="1">
         <v>1</v>
@@ -5826,28 +5826,28 @@
         <v>92</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>749</v>
+        <v>741</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>688</v>
+        <v>680</v>
       </c>
       <c r="O51" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="Q51" s="1">
         <v>1</v>
@@ -5876,10 +5876,10 @@
         <v>94</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>13</v>
@@ -5897,10 +5897,10 @@
         <v>95</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>481</v>
+        <v>778</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q52" s="1">
         <v>1</v>
@@ -5929,7 +5929,7 @@
         <v>97</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>98</v>
@@ -5950,10 +5950,10 @@
         <v>99</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>100</v>
+        <v>779</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q53" s="1">
         <v>1</v>
@@ -5973,19 +5973,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="E54" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>482</v>
+        <v>773</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>13</v>
@@ -6000,13 +6000,13 @@
         <v>13</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q54" s="1">
         <v>1</v>
@@ -6026,19 +6026,19 @@
         <v>54</v>
       </c>
       <c r="B55" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D55" s="1" t="s">
+      <c r="E55" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>13</v>
@@ -6053,13 +6053,13 @@
         <v>13</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="Q55" s="1">
         <v>1</v>
@@ -6079,19 +6079,19 @@
         <v>55</v>
       </c>
       <c r="B56" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="D56" s="1" t="s">
+      <c r="E56" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="F56" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>13</v>
@@ -6106,16 +6106,16 @@
         <v>13</v>
       </c>
       <c r="K56" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="O56" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="L56" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="O56" s="1" t="s">
-        <v>265</v>
-      </c>
       <c r="P56" s="1" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="Q56" s="1">
         <v>1</v>
@@ -6135,19 +6135,19 @@
         <v>56</v>
       </c>
       <c r="B57" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="E57" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>13</v>
@@ -6162,13 +6162,13 @@
         <v>13</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>487</v>
+        <v>781</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="Q57" s="1">
         <v>1</v>
@@ -6188,19 +6188,19 @@
         <v>57</v>
       </c>
       <c r="B58" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>114</v>
-      </c>
       <c r="E58" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>13</v>
@@ -6215,13 +6215,13 @@
         <v>13</v>
       </c>
       <c r="K58" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="L58" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="O58" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="O58" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="Q58" s="1">
         <v>1</v>
@@ -6241,19 +6241,19 @@
         <v>58</v>
       </c>
       <c r="B59" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="E59" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>13</v>
@@ -6268,13 +6268,13 @@
         <v>13</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q59" s="1">
         <v>1</v>
@@ -6294,19 +6294,19 @@
         <v>59</v>
       </c>
       <c r="B60" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="E60" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>13</v>
@@ -6321,16 +6321,16 @@
         <v>13</v>
       </c>
       <c r="K60" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="O60" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="L60" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="O60" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="P60" s="1" t="s">
-        <v>388</v>
+        <v>774</v>
       </c>
       <c r="Q60" s="1">
         <v>1</v>
@@ -6350,19 +6350,19 @@
         <v>60</v>
       </c>
       <c r="B61" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="E61" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>492</v>
+        <v>485</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>13</v>
@@ -6377,16 +6377,16 @@
         <v>13</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="O61" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="Q61" s="1">
         <v>1</v>
@@ -6406,19 +6406,19 @@
         <v>61</v>
       </c>
       <c r="B62" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="F62" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="E62" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="F62" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>13</v>
@@ -6433,16 +6433,16 @@
         <v>13</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P62" s="1" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="Q62" s="1">
         <v>1</v>
@@ -6462,19 +6462,19 @@
         <v>62</v>
       </c>
       <c r="B63" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D63" s="1" t="s">
+      <c r="E63" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F63" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>13</v>
@@ -6489,13 +6489,13 @@
         <v>13</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>497</v>
+        <v>490</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>778</v>
+        <v>768</v>
       </c>
       <c r="Q63" s="1">
         <v>1</v>
@@ -6515,31 +6515,31 @@
         <v>63</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="E64" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F64" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="J64" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="G64" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="H64" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="I64" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>272</v>
-      </c>
       <c r="O64" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="Q64" s="1">
         <v>1</v>
@@ -6559,31 +6559,31 @@
         <v>64</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="E65" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="G65" s="1" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="H65" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="I65" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="I65" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="J65" s="1" t="s">
-        <v>275</v>
+        <v>775</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="Q65" s="1">
         <v>1</v>
@@ -6603,31 +6603,31 @@
         <v>65</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="E66" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>750</v>
+        <v>742</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>689</v>
+        <v>681</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="Q66" s="1">
         <v>1</v>
@@ -6647,31 +6647,31 @@
         <v>66</v>
       </c>
       <c r="C67" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="E67" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>502</v>
+        <v>495</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>751</v>
+        <v>743</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="Q67" s="1">
         <v>1</v>
@@ -6691,31 +6691,31 @@
         <v>67</v>
       </c>
       <c r="C68" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D68" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="E68" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>752</v>
+        <v>744</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>505</v>
+        <v>498</v>
       </c>
       <c r="Q68" s="1">
         <v>1</v>
@@ -6735,31 +6735,31 @@
         <v>68</v>
       </c>
       <c r="C69" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="E69" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>753</v>
+        <v>745</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>754</v>
+        <v>746</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="Q69" s="1">
         <v>1</v>
@@ -6782,31 +6782,31 @@
         <v>69</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="E70" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="O70" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>755</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>591</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>639</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="O70" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="Q70" s="1">
         <v>1</v>
@@ -6829,34 +6829,34 @@
         <v>70</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>756</v>
+        <v>748</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>757</v>
+        <v>749</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>692</v>
+        <v>684</v>
       </c>
       <c r="N71" s="7">
         <v>1</v>
       </c>
       <c r="O71" s="1" t="s">
-        <v>779</v>
+        <v>769</v>
       </c>
       <c r="Q71" s="1">
         <v>1</v>
@@ -6879,31 +6879,31 @@
         <v>71</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D72" s="1" t="s">
+      <c r="E72" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E72" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>150</v>
-      </c>
       <c r="G72" s="1" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>640</v>
+        <v>633</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>759</v>
+        <v>751</v>
       </c>
       <c r="O72" s="1" t="s">
-        <v>780</v>
+        <v>770</v>
       </c>
       <c r="Q72" s="1">
         <v>1</v>
@@ -6926,31 +6926,31 @@
         <v>72</v>
       </c>
       <c r="C73" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="E73" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>693</v>
+        <v>685</v>
       </c>
       <c r="O73" s="1" t="s">
-        <v>781</v>
+        <v>771</v>
       </c>
       <c r="Q73" s="1">
         <v>1</v>
@@ -6973,31 +6973,31 @@
         <v>73</v>
       </c>
       <c r="C74" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="E74" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>761</v>
+        <v>753</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>762</v>
+        <v>754</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>763</v>
+        <v>755</v>
       </c>
       <c r="O74" s="1" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="Q74" s="1">
         <v>1</v>
@@ -7020,31 +7020,31 @@
         <v>74</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D75" s="1" t="s">
+      <c r="E75" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="F75" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E75" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="G75" s="1" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>694</v>
+        <v>686</v>
       </c>
       <c r="O75" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="Q75" s="1">
         <v>1</v>
@@ -7067,31 +7067,31 @@
         <v>75</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="E76" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>764</v>
+        <v>756</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>695</v>
+        <v>687</v>
       </c>
       <c r="O76" s="1" t="s">
-        <v>510</v>
+        <v>503</v>
       </c>
       <c r="Q76" s="1">
         <v>1</v>
@@ -7111,31 +7111,31 @@
         <v>76</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="D77" s="1" t="s">
-        <v>161</v>
-      </c>
       <c r="E77" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>765</v>
+        <v>757</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>643</v>
+        <v>636</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>766</v>
+        <v>776</v>
       </c>
       <c r="O77" s="1" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="Q77" s="1">
         <v>1</v>
@@ -7155,31 +7155,31 @@
         <v>77</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>163</v>
-      </c>
       <c r="E78" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>767</v>
+        <v>758</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>768</v>
+        <v>759</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>769</v>
+        <v>777</v>
       </c>
       <c r="O78" s="1" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="Q78" s="1">
         <v>1</v>
@@ -7199,31 +7199,31 @@
         <v>78</v>
       </c>
       <c r="C79" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D79" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="E79" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>645</v>
+        <v>638</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
       <c r="O79" s="1" t="s">
-        <v>512</v>
+        <v>505</v>
       </c>
       <c r="Q79" s="1">
         <v>1</v>
@@ -7243,31 +7243,31 @@
         <v>79</v>
       </c>
       <c r="C80" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="D80" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="E80" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>646</v>
+        <v>639</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>771</v>
+        <v>761</v>
       </c>
       <c r="O80" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q80" s="1">
         <v>1</v>
@@ -7287,31 +7287,31 @@
         <v>80</v>
       </c>
       <c r="C81" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="D81" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="E81" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>513</v>
+        <v>506</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>772</v>
+        <v>762</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>647</v>
+        <v>640</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
       <c r="O81" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q81" s="1">
         <v>1</v>
@@ -7334,31 +7334,31 @@
         <v>48</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>773</v>
+        <v>763</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>774</v>
+        <v>764</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
       <c r="M82" s="7">
         <v>1</v>
       </c>
       <c r="O82" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="Q82" s="1">
         <v>1</v>
@@ -7381,28 +7381,28 @@
         <v>69</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>775</v>
+        <v>765</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>648</v>
+        <v>641</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="O83" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="S83" s="1">
         <v>1</v>
@@ -7419,34 +7419,34 @@
         <v>20</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>46</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="I84" s="7" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
       <c r="J84" s="7" t="s">
-        <v>664</v>
+        <v>656</v>
       </c>
       <c r="M84" s="7">
         <v>1</v>
       </c>
       <c r="O84" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="Q84" s="7">
         <v>1</v>
@@ -7471,7 +7471,7 @@
     <sortCondition ref="C2:C81"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7496,7 +7496,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -8008,7 +8008,7 @@
         <v>63</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -8019,7 +8019,7 @@
         <v>64</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -8030,7 +8030,7 @@
         <v>65</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -8041,7 +8041,7 @@
         <v>83</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -8063,7 +8063,7 @@
         <v>66</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -8074,7 +8074,7 @@
         <v>67</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -8118,7 +8118,7 @@
         <v>68</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -8129,7 +8129,7 @@
         <v>69</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -8140,7 +8140,7 @@
         <v>70</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -8151,7 +8151,7 @@
         <v>71</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -8162,7 +8162,7 @@
         <v>72</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -8173,7 +8173,7 @@
         <v>73</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -8261,7 +8261,7 @@
         <v>74</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -8272,7 +8272,7 @@
         <v>75</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -8294,7 +8294,7 @@
         <v>76</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -8305,7 +8305,7 @@
         <v>77</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8456,7 +8456,7 @@
         <v>78</v>
       </c>
       <c r="D85" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="86" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8467,7 +8467,7 @@
         <v>79</v>
       </c>
       <c r="D86" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="87" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8478,7 +8478,7 @@
         <v>80</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="88" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8517,10 +8517,10 @@
         <v>53</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D90" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8531,10 +8531,10 @@
         <v>54</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="92" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8545,10 +8545,10 @@
         <v>55</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D92" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="93" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8559,10 +8559,10 @@
         <v>56</v>
       </c>
       <c r="C93" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D93" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="94" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8573,10 +8573,10 @@
         <v>57</v>
       </c>
       <c r="C94" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D94" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="95" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8587,10 +8587,10 @@
         <v>58</v>
       </c>
       <c r="C95" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D95" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="96" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8601,10 +8601,10 @@
         <v>59</v>
       </c>
       <c r="C96" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D96" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="97" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8615,10 +8615,10 @@
         <v>60</v>
       </c>
       <c r="C97" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D97" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="98" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8629,10 +8629,10 @@
         <v>61</v>
       </c>
       <c r="C98" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D98" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="99" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -8643,10 +8643,10 @@
         <v>62</v>
       </c>
       <c r="C99" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D99" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CANS-314: additional spelling fixes
</commit_message>
<xml_diff>
--- a/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank.xlsx
+++ b/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank.xlsx
@@ -2598,12 +2598,6 @@
     <t xml:space="preserve">Problems are dangerous or disabling; requires immediate and/or intensive action. Child/youth makes decisions that would likely result in significant physical harm to self or others. Therefore, youth requires intense and constant supervision, over and above that expected for the child/youth's age. </t>
   </si>
   <si>
-    <t xml:space="preserve">This item describes whether or not the child/youth has experienced verbal and/or nonverbal emotional abuse, including belittling, shaming, and humiliating a child/youth, calling names, making negative comparisons to others, or telling a child/youth that they are, "no good." This item includes both "emotional abuse," which would include psychological maltreatment such as insults or humiliation towards a child and "emotional neglect," described as the denial of emotional attention and/or support from caregivers. </t>
-  </si>
-  <si>
-    <t>Terrorism is defined as "the calculated use of violence or the threat of violence to inculcate fear, intended to coerce or to intimidate governments or societies in the pursuit of goals that are generally political, religious or ideological." Terrorism includes attacks by individuals acting in isolation (e.g. sniper attacks).</t>
-  </si>
-  <si>
     <t>Problems are dangerous or disabling; requires immediate and/or intensive action. Concern in two or more areas of regulation, including but not limited to: difficulties in breathing, body movements, crying, sleeping, feeding, attention, ability to self soothe, and/or sensitivity to environmental stressors.</t>
   </si>
   <si>
@@ -2628,6 +2622,12 @@
   </si>
   <si>
     <t>Child/youth has witnessed, or there is a suspicion that they witnessed family violence - single, repeated, or severe episodes. This includes episodes of family violence but no significant injuries (i.e. requiring emergency medical attention) and episodes in which significant injuries have occurred as a direct result of the violence.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This item describes whether or not the child/youth has experienced verbal and/or nonverbal emotional abuse, including belittling, shaming, and humiliating a child/youth, calling names, making negative comparisons to others, or telling a child/youth that they are, "no good". This item includes both "emotional abuse", which would include psychological maltreatment such as insults or humiliation towards a child and "emotional neglect", described as the denial of emotional attention and/or support from caregivers. </t>
+  </si>
+  <si>
+    <t>Terrorism is defined as "the calculated use of violence or the threat of violence to inculcate fear, intended to coerce or to intimidate governments or societies in the pursuit of goals that are generally political, religious or ideological". Terrorism includes attacks by individuals acting in isolation (e.g. sniper attacks).</t>
   </si>
 </sst>
 </file>
@@ -3513,10 +3513,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q2" sqref="Q2"/>
-      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
+      <selection pane="bottomLeft" activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5069,7 +5069,7 @@
         <v>279</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="Q34" s="1">
         <v>1</v>
@@ -5897,7 +5897,7 @@
         <v>95</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="O52" s="1" t="s">
         <v>260</v>
@@ -5950,7 +5950,7 @@
         <v>99</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="O53" s="1" t="s">
         <v>261</v>
@@ -5985,7 +5985,7 @@
         <v>339</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>773</v>
+        <v>780</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>13</v>
@@ -6165,7 +6165,7 @@
         <v>265</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="O57" s="1" t="s">
         <v>415</v>
@@ -6330,7 +6330,7 @@
         <v>120</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>774</v>
+        <v>781</v>
       </c>
       <c r="Q60" s="1">
         <v>1</v>
@@ -6580,7 +6580,7 @@
         <v>273</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="O65" s="1" t="s">
         <v>493</v>
@@ -7132,7 +7132,7 @@
         <v>636</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="O77" s="1" t="s">
         <v>427</v>
@@ -7176,7 +7176,7 @@
         <v>637</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="O78" s="1" t="s">
         <v>429</v>

</xml_diff>

<commit_message>
CANS-345: help tool tips added to Early Childhood domains
</commit_message>
<xml_diff>
--- a/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank.xlsx
+++ b/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="37680" yWindow="5595" windowWidth="28800" windowHeight="16680" tabRatio="555" activeTab="1"/>
+    <workbookView xWindow="37680" yWindow="5595" windowWidth="28800" windowHeight="16680" tabRatio="555"/>
   </bookViews>
   <sheets>
-    <sheet name="Domains" sheetId="4" r:id="rId1"/>
+    <sheet name="cans_domains" sheetId="4" r:id="rId1"/>
     <sheet name="cans_items" sheetId="2" r:id="rId2"/>
     <sheet name="Domain_Items" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">cans_items!$A$1:$X$83</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Domain_Items!$A$1:$D$41</definedName>
     <definedName name="_Toc328064535" localSheetId="1">cans_items!$I$3</definedName>
-    <definedName name="_Toc513575314" localSheetId="0">Domains!$B$4</definedName>
+    <definedName name="_Toc513575314" localSheetId="0">cans_domains!$B$4</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="787">
   <si>
     <t>Domain_ID</t>
   </si>
@@ -804,9 +804,6 @@
     <t>No evidence of any trauma of this type.</t>
   </si>
   <si>
-    <t>Child/youth has had experience or there is suspicion that the child/youth has experienced this type of trauma—one incident, multiple incidents, or chronic, on-going experiences.</t>
-  </si>
-  <si>
     <t>YN</t>
   </si>
   <si>
@@ -820,9 +817,6 @@
   </si>
   <si>
     <t>RISK BEHAVIORS &amp; FACTORS</t>
-  </si>
-  <si>
-    <t>CULTURAL FACTORS – FAMILY</t>
   </si>
   <si>
     <t xml:space="preserve">No current need; no need for action or intervention. </t>
@@ -2628,6 +2622,27 @@
   </si>
   <si>
     <t>No current need; no need for action or intervention. Strong evidence the child is developing strong self-capacities. This is indicated by the capacity to fall asleep, regular patterns of feeding and sleeping. Young infants can regulate breathing and body temperature, are able to move smoothly between states of alertness, sleep, feeding on schedule, able to make use of caregiver/pacifier to be soothed, and moving toward regulating themselves (e.g., infant can begin to calm to caregiver's voice prior to being picked up). Toddlers are able to make use of caregiver to help regulate emotions, fall asleep with appropriate transitional objects, can attend to play with increased attention and play is becoming more elaborated, or have some ability to calm themselves down.</t>
+  </si>
+  <si>
+    <t>This section focuses on identifying the child's social/emotional or behavioral challenges.</t>
+  </si>
+  <si>
+    <t>These items identify linguistic or cultural issues for which service providers need to make accommodations. Items in the Cultural Factors Domain describe difficulties that the child's family experiences or encounters as a result of their membership in any cultural group, and/or because of the relationship between members of that group and members of the dominant society. In rating these items, please use the perspective of the child's family.</t>
+  </si>
+  <si>
+    <t>This section considers factors that impact the ways in which the caregiver/child dyad interacts. There is nothing that has more impact on a child than the way that their parent or caregiver interacts with them. The dyadic interaction that is supportive allows for the child to focus fully on growth and development. It is the foundation for the development of all other social relationships and guides and supports all areas of development.</t>
+  </si>
+  <si>
+    <t>This section focuses primarily on the various developmental domains and functioning of the child in a variety of settings including the home, school and community. For items in this section, it may be helpful to ask the general question, "Do you have any concerns in this area?"</t>
+  </si>
+  <si>
+    <t>Risk behaviors are actions that can get children in trouble or put them in danger of harming themselves or others. This section also includes factors that may place the child's development at risk.</t>
+  </si>
+  <si>
+    <t>CULTURAL FACTORS - FAMILY</t>
+  </si>
+  <si>
+    <t>Child/youth has had experience or there is suspicion that the child/youth has experienced this type of trauma-one incident, multiple incidents, or chronic, on-going experiences.</t>
   </si>
 </sst>
 </file>
@@ -3019,8 +3034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3058,7 +3073,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>221</v>
@@ -3079,7 +3094,7 @@
         <v>226</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -3090,13 +3105,13 @@
         <v>198</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="G2" s="4">
         <v>1</v>
@@ -3125,7 +3140,7 @@
         <v>204</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>205</v>
@@ -3160,13 +3175,13 @@
         <v>207</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G4" s="4">
         <v>1</v>
@@ -3195,13 +3210,13 @@
         <v>208</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G5" s="4">
         <v>1</v>
@@ -3230,10 +3245,10 @@
         <v>210</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>211</v>
@@ -3265,13 +3280,13 @@
         <v>216</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
@@ -3306,10 +3321,10 @@
         <v>219</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>220</v>
@@ -3324,10 +3339,10 @@
         <v>227</v>
       </c>
       <c r="N8" s="4" t="s">
+        <v>786</v>
+      </c>
+      <c r="O8" s="4" t="s">
         <v>228</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -3335,10 +3350,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>780</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
@@ -3364,10 +3382,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>783</v>
       </c>
       <c r="F10" s="4">
         <v>1</v>
@@ -3393,10 +3414,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>784</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
@@ -3422,16 +3446,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>234</v>
+        <v>785</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>781</v>
       </c>
       <c r="F12" s="4">
         <v>1</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>202</v>
@@ -3451,10 +3478,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>513</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
@@ -3480,10 +3510,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>782</v>
       </c>
       <c r="F14" s="4">
         <v>1</v>
@@ -3513,10 +3546,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q2" sqref="Q2"/>
-      <selection pane="bottomLeft" activeCell="K57" sqref="K57"/>
+      <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3545,7 +3578,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -3557,7 +3590,7 @@
         <v>200</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -3581,16 +3614,16 @@
         <v>226</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>199</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>4</v>
@@ -3605,7 +3638,7 @@
         <v>6</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>169</v>
@@ -3628,28 +3661,28 @@
         <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="S2" s="1">
         <v>1</v>
@@ -3672,22 +3705,22 @@
         <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>16</v>
@@ -3719,22 +3752,22 @@
         <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>19</v>
@@ -3766,22 +3799,22 @@
         <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>22</v>
@@ -3813,25 +3846,25 @@
         <v>24</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H6" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>692</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>694</v>
-      </c>
       <c r="O6" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="Q6" s="1">
         <v>1</v>
@@ -3857,22 +3890,22 @@
         <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>27</v>
@@ -3898,22 +3931,22 @@
         <v>28</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="N8" s="7">
         <v>1</v>
@@ -3945,22 +3978,22 @@
         <v>30</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>31</v>
@@ -3989,25 +4022,25 @@
         <v>33</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="Q10" s="1">
         <v>1</v>
@@ -4036,22 +4069,22 @@
         <v>36</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>172</v>
@@ -4080,25 +4113,25 @@
         <v>37</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="R12" s="1">
         <v>1</v>
@@ -4121,22 +4154,22 @@
         <v>38</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>173</v>
@@ -4165,25 +4198,25 @@
         <v>40</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="Q14" s="1">
         <v>1</v>
@@ -4206,28 +4239,28 @@
         <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="R15" s="1">
         <v>1</v>
@@ -4250,25 +4283,25 @@
         <v>41</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="H16" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>705</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>706</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>707</v>
-      </c>
       <c r="O16" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="R16" s="1">
         <v>1</v>
@@ -4291,25 +4324,25 @@
         <v>42</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="R17" s="1">
         <v>1</v>
@@ -4332,22 +4365,22 @@
         <v>43</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>174</v>
@@ -4376,25 +4409,25 @@
         <v>45</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="R19" s="1">
         <v>1</v>
@@ -4414,28 +4447,28 @@
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="R20" s="1">
         <v>1</v>
@@ -4455,28 +4488,28 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>175</v>
@@ -4505,25 +4538,25 @@
         <v>47</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>453</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>455</v>
-      </c>
       <c r="J22" s="1" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="R22" s="1">
         <v>1</v>
@@ -4549,22 +4582,22 @@
         <v>49</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>176</v>
@@ -4593,22 +4626,22 @@
         <v>50</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>177</v>
@@ -4637,22 +4670,22 @@
         <v>51</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>178</v>
@@ -4681,22 +4714,22 @@
         <v>52</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>179</v>
@@ -4725,22 +4758,22 @@
         <v>53</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>180</v>
@@ -4769,22 +4802,22 @@
         <v>54</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>181</v>
@@ -4816,22 +4849,22 @@
         <v>55</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>182</v>
@@ -4860,25 +4893,25 @@
         <v>57</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="Q30" s="1">
         <v>1</v>
@@ -4907,22 +4940,22 @@
         <v>60</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>183</v>
@@ -4954,25 +4987,25 @@
         <v>62</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="Q32" s="1">
         <v>1</v>
@@ -5001,25 +5034,25 @@
         <v>64</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="Q33" s="1">
         <v>1</v>
@@ -5048,28 +5081,28 @@
         <v>66</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="Q34" s="1">
         <v>1</v>
@@ -5095,28 +5128,28 @@
         <v>67</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="M35" s="7">
         <v>1</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="R35" s="1">
         <v>1</v>
@@ -5136,25 +5169,25 @@
         <v>35</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>68</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="O36" s="1" t="s">
         <v>184</v>
@@ -5180,25 +5213,25 @@
         <v>70</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="R37" s="1">
         <v>1</v>
@@ -5221,22 +5254,22 @@
         <v>71</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="O38" s="1" t="s">
         <v>185</v>
@@ -5262,22 +5295,22 @@
         <v>72</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="O39" s="1" t="s">
         <v>186</v>
@@ -5303,25 +5336,25 @@
         <v>73</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="O40" s="1" t="s">
         <v>187</v>
@@ -5350,25 +5383,25 @@
         <v>75</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="O41" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="Q41" s="1">
         <v>1</v>
@@ -5397,25 +5430,25 @@
         <v>77</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="O42" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="Q42" s="1">
         <v>1</v>
@@ -5444,22 +5477,22 @@
         <v>79</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="O43" s="1" t="s">
         <v>188</v>
@@ -5491,28 +5524,28 @@
         <v>81</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="Q44" s="1">
         <v>1</v>
@@ -5541,22 +5574,22 @@
         <v>83</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="O45" s="1" t="s">
         <v>189</v>
@@ -5585,28 +5618,28 @@
         <v>84</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="Q46" s="1">
         <v>1</v>
@@ -5635,25 +5668,25 @@
         <v>45</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="Q47" s="1">
         <v>1</v>
@@ -5682,25 +5715,25 @@
         <v>87</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="Q48" s="1">
         <v>1</v>
@@ -5729,22 +5762,22 @@
         <v>28</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>89</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="N49" s="7">
         <v>1</v>
@@ -5782,25 +5815,25 @@
         <v>91</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="Q50" s="1">
         <v>1</v>
@@ -5826,25 +5859,25 @@
         <v>92</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="O51" s="1" t="s">
         <v>191</v>
@@ -5876,10 +5909,10 @@
         <v>94</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>13</v>
@@ -5897,10 +5930,10 @@
         <v>95</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="Q52" s="1">
         <v>1</v>
@@ -5929,7 +5962,7 @@
         <v>97</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>98</v>
@@ -5950,10 +5983,10 @@
         <v>99</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="Q53" s="1">
         <v>1</v>
@@ -5982,10 +6015,10 @@
         <v>101</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>13</v>
@@ -6003,10 +6036,10 @@
         <v>102</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="O54" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="Q54" s="1">
         <v>1</v>
@@ -6035,7 +6068,7 @@
         <v>104</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>105</v>
@@ -6056,10 +6089,10 @@
         <v>106</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="Q55" s="1">
         <v>1</v>
@@ -6088,7 +6121,7 @@
         <v>108</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>109</v>
@@ -6106,16 +6139,16 @@
         <v>13</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="L56" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="Q56" s="1">
         <v>1</v>
@@ -6144,10 +6177,10 @@
         <v>111</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>13</v>
@@ -6162,13 +6195,13 @@
         <v>13</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L57" s="1" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="Q57" s="1">
         <v>1</v>
@@ -6197,10 +6230,10 @@
         <v>113</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>13</v>
@@ -6215,13 +6248,13 @@
         <v>13</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="O58" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="Q58" s="1">
         <v>1</v>
@@ -6250,10 +6283,10 @@
         <v>115</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>13</v>
@@ -6268,10 +6301,10 @@
         <v>13</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="O59" s="1" t="s">
         <v>116</v>
@@ -6303,10 +6336,10 @@
         <v>118</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="G60" s="1" t="s">
         <v>13</v>
@@ -6324,13 +6357,13 @@
         <v>119</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="O60" s="1" t="s">
         <v>120</v>
       </c>
       <c r="P60" s="1" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="Q60" s="1">
         <v>1</v>
@@ -6359,10 +6392,10 @@
         <v>122</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>13</v>
@@ -6380,13 +6413,13 @@
         <v>123</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="O61" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="P61" s="1" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="Q61" s="1">
         <v>1</v>
@@ -6412,10 +6445,10 @@
         <v>124</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>125</v>
@@ -6436,13 +6469,13 @@
         <v>126</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="O62" s="1" t="s">
         <v>192</v>
       </c>
       <c r="P62" s="1" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="Q62" s="1">
         <v>1</v>
@@ -6471,7 +6504,7 @@
         <v>128</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>129</v>
@@ -6489,13 +6522,13 @@
         <v>13</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="Q63" s="1">
         <v>1</v>
@@ -6521,25 +6554,25 @@
         <v>131</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="O64" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="Q64" s="1">
         <v>1</v>
@@ -6565,25 +6598,25 @@
         <v>133</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>134</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="O65" s="1" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="Q65" s="1">
         <v>1</v>
@@ -6609,25 +6642,25 @@
         <v>136</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="Q66" s="1">
         <v>1</v>
@@ -6653,25 +6686,25 @@
         <v>138</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="O67" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="Q67" s="1">
         <v>1</v>
@@ -6697,25 +6730,25 @@
         <v>140</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F68" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="I68" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="O68" s="1" t="s">
         <v>495</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>496</v>
-      </c>
-      <c r="H68" s="1" t="s">
-        <v>582</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="J68" s="1" t="s">
-        <v>743</v>
-      </c>
-      <c r="O68" s="1" t="s">
-        <v>497</v>
       </c>
       <c r="Q68" s="1">
         <v>1</v>
@@ -6741,25 +6774,25 @@
         <v>142</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="Q69" s="1">
         <v>1</v>
@@ -6788,22 +6821,22 @@
         <v>144</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="O70" s="1" t="s">
         <v>145</v>
@@ -6835,28 +6868,28 @@
         <v>8</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="N71" s="7">
         <v>1</v>
       </c>
       <c r="O71" s="1" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="Q71" s="1">
         <v>1</v>
@@ -6885,25 +6918,25 @@
         <v>148</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>149</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="O72" s="1" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="Q72" s="1">
         <v>1</v>
@@ -6932,25 +6965,25 @@
         <v>151</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="O73" s="1" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="Q73" s="1">
         <v>1</v>
@@ -6979,25 +7012,25 @@
         <v>153</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="G74" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="J74" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="H74" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="J74" s="1" t="s">
-        <v>754</v>
-      </c>
       <c r="O74" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="Q74" s="1">
         <v>1</v>
@@ -7026,25 +7059,25 @@
         <v>155</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>156</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="O75" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="Q75" s="1">
         <v>1</v>
@@ -7073,25 +7106,25 @@
         <v>158</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="O76" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="Q76" s="1">
         <v>1</v>
@@ -7117,25 +7150,25 @@
         <v>160</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="O77" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="Q77" s="1">
         <v>1</v>
@@ -7161,25 +7194,25 @@
         <v>162</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="O78" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="Q78" s="1">
         <v>1</v>
@@ -7205,25 +7238,25 @@
         <v>164</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="O79" s="1" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="Q79" s="1">
         <v>1</v>
@@ -7249,22 +7282,22 @@
         <v>166</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="O80" s="1" t="s">
         <v>193</v>
@@ -7293,22 +7326,22 @@
         <v>168</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="O81" s="1" t="s">
         <v>194</v>
@@ -7334,31 +7367,31 @@
         <v>48</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="M82" s="7">
         <v>1</v>
       </c>
       <c r="O82" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="Q82" s="1">
         <v>1</v>
@@ -7381,28 +7414,28 @@
         <v>69</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="J83" s="1" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="O83" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="S83" s="1">
         <v>1</v>
@@ -7419,28 +7452,28 @@
         <v>20</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>46</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="G84" s="7" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="H84" s="7" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="I84" s="7" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J84" s="7" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="M84" s="7">
         <v>1</v>
@@ -7496,7 +7529,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -8041,7 +8074,7 @@
         <v>83</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CANS-344: EC.18 not confidential by default
</commit_message>
<xml_diff>
--- a/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank.xlsx
+++ b/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="37680" yWindow="5595" windowWidth="28800" windowHeight="16680" tabRatio="555"/>
+    <workbookView xWindow="0" yWindow="5595" windowWidth="20295" windowHeight="795" tabRatio="555" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cans_domains" sheetId="4" r:id="rId1"/>
@@ -3034,8 +3034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3546,10 +3546,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X84"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q2" sqref="Q2"/>
-      <selection pane="bottomLeft" activeCell="F56" sqref="F56"/>
+      <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6884,9 +6884,6 @@
       </c>
       <c r="J71" s="1" t="s">
         <v>681</v>
-      </c>
-      <c r="N71" s="7">
-        <v>1</v>
       </c>
       <c r="O71" s="1" t="s">
         <v>766</v>

</xml_diff>

<commit_message>
CANS-683. Add text description next to N/A on specific questions in CANS Assessment Form
</commit_message>
<xml_diff>
--- a/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank.xlsx
+++ b/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amerabelay/cwds/abelayt/cans/pi10/spr10-1/cans-api-340-refactor-domain-title/cans-api/tools/instrument-parser/csv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/metquota/cwds/cans-api/tools/instrument-parser/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8FD2CB-63CD-8F4A-A1D2-175E70EDB344}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22780" tabRatio="555"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16660" tabRatio="555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cans_domains" sheetId="4" r:id="rId1"/>
@@ -22,23 +23,23 @@
     <definedName name="_Toc328064535" localSheetId="1">cans_items!$I$3</definedName>
     <definedName name="_Toc513575314" localSheetId="0">cans_domains!$B$4</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="787">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="789">
   <si>
     <t>Domain_ID</t>
   </si>
@@ -2650,11 +2651,17 @@
   <si>
     <t>Dyadic Considerations</t>
   </si>
+  <si>
+    <t>Youth is not in school</t>
+  </si>
+  <si>
+    <t>Child is younger than 12 months of age</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3037,10 +3044,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3206,7 +3213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="409" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3547,13 +3554,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X84"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="84" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q2" sqref="Q2"/>
-      <selection pane="bottomLeft" activeCell="I71" sqref="I71"/>
+      <selection pane="bottomLeft" activeCell="M84" sqref="M84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="27" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3565,10 +3572,12 @@
     <col min="5" max="5" width="28.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="32.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="20.83203125" style="1" customWidth="1"/>
-    <col min="8" max="10" width="7.6640625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="7.6640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.83203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="23.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="7.6640625" style="1" customWidth="1"/>
-    <col min="13" max="14" width="7.6640625" style="7" customWidth="1"/>
+    <col min="13" max="13" width="22" style="7" customWidth="1"/>
+    <col min="14" max="14" width="7.6640625" style="7" customWidth="1"/>
     <col min="15" max="15" width="93.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="18" width="7.6640625" style="1" customWidth="1"/>
     <col min="19" max="19" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -5149,8 +5158,8 @@
       <c r="J35" s="1" t="s">
         <v>652</v>
       </c>
-      <c r="M35" s="7">
-        <v>1</v>
+      <c r="M35" s="7" t="s">
+        <v>787</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>389</v>
@@ -7360,7 +7369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:23" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -7388,8 +7397,8 @@
       <c r="J82" s="1" t="s">
         <v>674</v>
       </c>
-      <c r="M82" s="7">
-        <v>1</v>
+      <c r="M82" s="7" t="s">
+        <v>788</v>
       </c>
       <c r="O82" s="1" t="s">
         <v>417</v>
@@ -7445,7 +7454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:23" s="7" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:23" s="7" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="7">
         <v>83</v>
       </c>
@@ -7476,8 +7485,8 @@
       <c r="J84" s="7" t="s">
         <v>641</v>
       </c>
-      <c r="M84" s="7">
-        <v>1</v>
+      <c r="M84" s="7" t="s">
+        <v>788</v>
       </c>
       <c r="O84" s="7" t="s">
         <v>175</v>
@@ -7496,7 +7505,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X83">
+  <autoFilter ref="A1:X83" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState ref="A2:X83">
       <sortCondition ref="A1:A83"/>
     </sortState>
@@ -7510,7 +7519,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D99"/>
   <sheetViews>
     <sheetView topLeftCell="A51" workbookViewId="0">
@@ -7525,7 +7534,7 @@
     <col min="5" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -7979,7 +7988,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>8</v>
       </c>
@@ -7990,7 +7999,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>8</v>
       </c>
@@ -8001,7 +8010,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>8</v>
       </c>
@@ -8012,7 +8021,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>8</v>
       </c>
@@ -8023,7 +8032,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>8</v>
       </c>
@@ -8034,7 +8043,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>8</v>
       </c>
@@ -8045,7 +8054,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>8</v>
       </c>
@@ -8056,7 +8065,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>8</v>
       </c>
@@ -8067,7 +8076,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>8</v>
       </c>
@@ -8078,7 +8087,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>9</v>
       </c>
@@ -8089,7 +8098,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>9</v>
       </c>
@@ -8100,7 +8109,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>9</v>
       </c>
@@ -8111,7 +8120,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>9</v>
       </c>
@@ -8122,7 +8131,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>9</v>
       </c>
@@ -8133,7 +8142,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>10</v>
       </c>
@@ -8144,7 +8153,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>10</v>
       </c>
@@ -8155,7 +8164,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>10</v>
       </c>
@@ -8166,7 +8175,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>10</v>
       </c>
@@ -8177,7 +8186,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>10</v>
       </c>
@@ -8188,7 +8197,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>10</v>
       </c>
@@ -8199,7 +8208,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>10</v>
       </c>
@@ -8210,7 +8219,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>11</v>
       </c>
@@ -8221,7 +8230,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>11</v>
       </c>
@@ -8232,7 +8241,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>11</v>
       </c>
@@ -8243,7 +8252,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>12</v>
       </c>
@@ -8254,7 +8263,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>12</v>
       </c>
@@ -8265,7 +8274,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>12</v>
       </c>
@@ -8276,7 +8285,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>12</v>
       </c>
@@ -8287,7 +8296,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>12</v>
       </c>
@@ -8298,7 +8307,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>12</v>
       </c>
@@ -8309,7 +8318,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>12</v>
       </c>
@@ -8320,7 +8329,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>13</v>
       </c>
@@ -8331,7 +8340,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>13</v>
       </c>
@@ -8342,7 +8351,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="75" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A75" s="8">
         <v>6</v>
       </c>
@@ -8356,7 +8365,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="8">
         <v>6</v>
       </c>
@@ -8370,7 +8379,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="77" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="8">
         <v>6</v>
       </c>
@@ -8384,7 +8393,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="8">
         <v>6</v>
       </c>
@@ -8398,7 +8407,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="8">
         <v>6</v>
       </c>
@@ -8412,7 +8421,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="8">
         <v>6</v>
       </c>
@@ -8426,7 +8435,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="8">
         <v>6</v>
       </c>
@@ -8440,7 +8449,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="8">
         <v>6</v>
       </c>
@@ -8454,7 +8463,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="8">
         <v>6</v>
       </c>
@@ -8468,7 +8477,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="8">
         <v>6</v>
       </c>
@@ -8482,7 +8491,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="85" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="8">
         <v>6</v>
       </c>
@@ -8493,7 +8502,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="86" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="8">
         <v>6</v>
       </c>
@@ -8504,7 +8513,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="87" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="8">
         <v>6</v>
       </c>
@@ -8515,7 +8524,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="88" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="8">
         <v>7</v>
       </c>
@@ -8529,7 +8538,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="89" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="8">
         <v>7</v>
       </c>
@@ -8543,7 +8552,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="90" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="8">
         <v>7</v>
       </c>
@@ -8557,7 +8566,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="8">
         <v>7</v>
       </c>
@@ -8571,7 +8580,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="8">
         <v>7</v>
       </c>
@@ -8585,7 +8594,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="93" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="8">
         <v>7</v>
       </c>
@@ -8599,7 +8608,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="94" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="8">
         <v>7</v>
       </c>
@@ -8613,7 +8622,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="95" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="8">
         <v>7</v>
       </c>
@@ -8627,7 +8636,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="96" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="8">
         <v>7</v>
       </c>
@@ -8641,7 +8650,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="97" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="8">
         <v>7</v>
       </c>
@@ -8655,7 +8664,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="98" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="8">
         <v>7</v>
       </c>
@@ -8669,7 +8678,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="99" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="8">
         <v>7</v>
       </c>
@@ -8684,7 +8693,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D41">
+  <autoFilter ref="A1:D41" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <sortState ref="A2:D41">
       <sortCondition ref="A1:A41"/>
     </sortState>

</xml_diff>

<commit_message>
edited the Domains excel sheet and exported it to csv file
</commit_message>
<xml_diff>
--- a/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank.xlsx
+++ b/tools/instrument-parser/csv/ANNOTATED_CANS ItemBank.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/metquota/cwds/cans-api/tools/instrument-parser/csv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amerabelay/cwds/abelayt/cans/pi11/spr11-2/cans-api-879-fix-domain-names/cans-api/tools/instrument-parser/csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8FD2CB-63CD-8F4A-A1D2-175E70EDB344}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16660" tabRatio="555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" tabRatio="555"/>
   </bookViews>
   <sheets>
     <sheet name="cans_domains" sheetId="4" r:id="rId1"/>
@@ -23,23 +22,23 @@
     <definedName name="_Toc328064535" localSheetId="1">cans_items!$I$3</definedName>
     <definedName name="_Toc513575314" localSheetId="0">cans_domains!$B$4</definedName>
   </definedNames>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1009" uniqueCount="788">
   <si>
     <t>Domain_ID</t>
   </si>
@@ -2631,37 +2630,34 @@
     <t>Caregiver Resources And Needs Domain</t>
   </si>
   <si>
-    <t>Potentially Traumatic / Adverse Childhood Experiences</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Challenges </t>
-  </si>
-  <si>
-    <t>Functioning</t>
-  </si>
-  <si>
-    <t>Risk Behaviors &amp; Factors</t>
-  </si>
-  <si>
-    <t>Cultural Factors - Family</t>
-  </si>
-  <si>
-    <t>Strengths</t>
-  </si>
-  <si>
-    <t>Dyadic Considerations</t>
-  </si>
-  <si>
     <t>Youth is not in school</t>
   </si>
   <si>
     <t>Child is younger than 12 months of age</t>
+  </si>
+  <si>
+    <t>Potentially Traumatic / Adverse Childhood Experiences Domain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Challenges Domain </t>
+  </si>
+  <si>
+    <t>Functioning Domain</t>
+  </si>
+  <si>
+    <t>Risk Behaviors &amp; Factors Domain</t>
+  </si>
+  <si>
+    <t>Cultural Factors - Family Domain</t>
+  </si>
+  <si>
+    <t>Dyadic Considerations Domain</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3044,15 +3040,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.6640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="4" customWidth="1"/>
@@ -3213,7 +3211,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="409" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -3329,7 +3327,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>275</v>
@@ -3361,7 +3359,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>276</v>
@@ -3393,7 +3391,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>278</v>
@@ -3425,7 +3423,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>279</v>
@@ -3457,7 +3455,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>277</v>
@@ -3489,7 +3487,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>785</v>
+        <v>778</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>280</v>
@@ -3521,7 +3519,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>281</v>
@@ -3554,10 +3552,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="84" workbookViewId="0">
+    <sheetView zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="84" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q2" sqref="Q2"/>
       <selection pane="bottomLeft" activeCell="M84" sqref="M84"/>
@@ -5159,7 +5157,7 @@
         <v>652</v>
       </c>
       <c r="M35" s="7" t="s">
-        <v>787</v>
+        <v>780</v>
       </c>
       <c r="O35" s="1" t="s">
         <v>389</v>
@@ -7398,7 +7396,7 @@
         <v>674</v>
       </c>
       <c r="M82" s="7" t="s">
-        <v>788</v>
+        <v>781</v>
       </c>
       <c r="O82" s="1" t="s">
         <v>417</v>
@@ -7486,7 +7484,7 @@
         <v>641</v>
       </c>
       <c r="M84" s="7" t="s">
-        <v>788</v>
+        <v>781</v>
       </c>
       <c r="O84" s="7" t="s">
         <v>175</v>
@@ -7505,7 +7503,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X83" xr:uid="{00000000-0009-0000-0000-000001000000}">
+  <autoFilter ref="A1:X83">
     <sortState ref="A2:X83">
       <sortCondition ref="A1:A83"/>
     </sortState>
@@ -7519,7 +7517,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D99"/>
   <sheetViews>
     <sheetView topLeftCell="A51" workbookViewId="0">
@@ -7534,7 +7532,7 @@
     <col min="5" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -7988,7 +7986,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>8</v>
       </c>
@@ -7999,7 +7997,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>8</v>
       </c>
@@ -8010,7 +8008,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>8</v>
       </c>
@@ -8021,7 +8019,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>8</v>
       </c>
@@ -8032,7 +8030,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>8</v>
       </c>
@@ -8043,7 +8041,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>8</v>
       </c>
@@ -8054,7 +8052,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>8</v>
       </c>
@@ -8065,7 +8063,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>8</v>
       </c>
@@ -8076,7 +8074,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>8</v>
       </c>
@@ -8087,7 +8085,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>9</v>
       </c>
@@ -8098,7 +8096,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>9</v>
       </c>
@@ -8109,7 +8107,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>9</v>
       </c>
@@ -8120,7 +8118,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>9</v>
       </c>
@@ -8131,7 +8129,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>9</v>
       </c>
@@ -8142,7 +8140,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>10</v>
       </c>
@@ -8153,7 +8151,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>10</v>
       </c>
@@ -8164,7 +8162,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>10</v>
       </c>
@@ -8175,7 +8173,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>10</v>
       </c>
@@ -8186,7 +8184,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>10</v>
       </c>
@@ -8197,7 +8195,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>10</v>
       </c>
@@ -8208,7 +8206,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>10</v>
       </c>
@@ -8219,7 +8217,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>11</v>
       </c>
@@ -8230,7 +8228,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>11</v>
       </c>
@@ -8241,7 +8239,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>11</v>
       </c>
@@ -8252,7 +8250,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>12</v>
       </c>
@@ -8263,7 +8261,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>12</v>
       </c>
@@ -8274,7 +8272,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>12</v>
       </c>
@@ -8285,7 +8283,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>12</v>
       </c>
@@ -8296,7 +8294,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>12</v>
       </c>
@@ -8307,7 +8305,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>12</v>
       </c>
@@ -8318,7 +8316,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>12</v>
       </c>
@@ -8329,7 +8327,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>13</v>
       </c>
@@ -8340,7 +8338,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>13</v>
       </c>
@@ -8351,7 +8349,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="75" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="8">
         <v>6</v>
       </c>
@@ -8365,7 +8363,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="76" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="8">
         <v>6</v>
       </c>
@@ -8379,7 +8377,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="77" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="8">
         <v>6</v>
       </c>
@@ -8393,7 +8391,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="8">
         <v>6</v>
       </c>
@@ -8407,7 +8405,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="8">
         <v>6</v>
       </c>
@@ -8421,7 +8419,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="80" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="8">
         <v>6</v>
       </c>
@@ -8435,7 +8433,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="81" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="8">
         <v>6</v>
       </c>
@@ -8449,7 +8447,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="8">
         <v>6</v>
       </c>
@@ -8463,7 +8461,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="83" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="8">
         <v>6</v>
       </c>
@@ -8477,7 +8475,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="8">
         <v>6</v>
       </c>
@@ -8491,7 +8489,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="85" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="8">
         <v>6</v>
       </c>
@@ -8502,7 +8500,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="86" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="8">
         <v>6</v>
       </c>
@@ -8513,7 +8511,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="87" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A87" s="8">
         <v>6</v>
       </c>
@@ -8524,7 +8522,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="88" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="8">
         <v>7</v>
       </c>
@@ -8538,7 +8536,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="89" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A89" s="8">
         <v>7</v>
       </c>
@@ -8552,7 +8550,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="90" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="8">
         <v>7</v>
       </c>
@@ -8566,7 +8564,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="8">
         <v>7</v>
       </c>
@@ -8580,7 +8578,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="8">
         <v>7</v>
       </c>
@@ -8594,7 +8592,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="93" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="8">
         <v>7</v>
       </c>
@@ -8608,7 +8606,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="94" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="8">
         <v>7</v>
       </c>
@@ -8622,7 +8620,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="95" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="8">
         <v>7</v>
       </c>
@@ -8636,7 +8634,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="96" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="8">
         <v>7</v>
       </c>
@@ -8650,7 +8648,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="97" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A97" s="8">
         <v>7</v>
       </c>
@@ -8664,7 +8662,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="98" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A98" s="8">
         <v>7</v>
       </c>
@@ -8678,7 +8676,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="99" spans="1:4" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A99" s="8">
         <v>7</v>
       </c>
@@ -8693,7 +8691,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D41" xr:uid="{00000000-0009-0000-0000-000002000000}">
+  <autoFilter ref="A1:D41">
     <sortState ref="A2:D41">
       <sortCondition ref="A1:A41"/>
     </sortState>

</xml_diff>